<commit_message>
ACINS-1679 Importer spec completed and bugs fixed.
</commit_message>
<xml_diff>
--- a/spec/fixtures/gpa_data.xlsx
+++ b/spec/fixtures/gpa_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1100" windowWidth="26840" windowHeight="15940"/>
+    <workbookView xWindow="3420" yWindow="1100" windowWidth="29380" windowHeight="18860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Course GPA</t>
   </si>
   <si>
-    <t>AFAM 102.001</t>
-  </si>
-  <si>
     <t>CRIM 111.002</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>def456</t>
+  </si>
+  <si>
+    <t>AFAM 102C.001</t>
   </si>
 </sst>
 </file>
@@ -203,16 +203,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,85 +541,85 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>2181</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>38</v>
@@ -666,13 +666,13 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>2181</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>45</v>
@@ -719,13 +719,13 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>2181</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>17</v>

</xml_diff>

<commit_message>
changed gpa header image in docs.  GPA importer using campus from file to import campus data to GPA, also is expecting there to only be one row of headers.  Fixed specs to mirror this.  Removed unecessary check in integration spec for the proper xml output.  Updated fixture for gpa specs.
</commit_message>
<xml_diff>
--- a/spec/fixtures/gpa_data.xlsx
+++ b/spec/fixtures/gpa_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajk5603/RubymineProjects/ai_integration/spec/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajk5603/RubymineProjects/fams_tools/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234141F9-67C9-6F47-B991-2CB8C29139B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1100" windowWidth="29380" windowHeight="18860"/>
+    <workbookView xWindow="3420" yWindow="820" windowWidth="29380" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>Grade Distribution</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Course &amp; Sect(s)</t>
   </si>
@@ -93,12 +91,21 @@
   </si>
   <si>
     <t>AFAM 102C.001</t>
+  </si>
+  <si>
+    <t>Campus</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>WC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -128,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,26 +160,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -192,32 +179,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="2"/>
-    <cellStyle name="Normal_Sheet1_1" xfId="1"/>
+    <cellStyle name="Normal_Sheet1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_Sheet1_1" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -528,252 +505,238 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>2181</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>38</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>12</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>2181</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>2181</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>2181</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>38</v>
-      </c>
-      <c r="E3">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>1</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>12</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>3.16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4">
-        <v>2181</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>45</v>
-      </c>
-      <c r="E4">
-        <v>16</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>7</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q4">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>2181</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>3.14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:Q1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>